<commit_message>
add new sheet to SED-BIOME data entry spreadsheets
</commit_message>
<xml_diff>
--- a/assets/projects/sed-biome/data-entry-spreadsheets/SED-BIOME_site-10_Australia.xlsx
+++ b/assets/projects/sed-biome/data-entry-spreadsheets/SED-BIOME_site-10_Australia.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlonn\Documents\Repositories\protocols\sed-biome\data_entry_spreadsheets\output_spreadsheets_noPI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lonnemanm\Documents\repositories\marinegeo.github.io\assets\projects\sed-biome\data-entry-spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED9CFE42-E4AA-4728-B861-4900C63F972B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B47B8A9-0685-4557-B0EF-08CFA6C68497}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2685" yWindow="2685" windowWidth="28800" windowHeight="15555" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="protocol_metadata" sheetId="1" r:id="rId1"/>
@@ -18,11 +18,12 @@
     <sheet name="minicore_and_syringe_metadata" sheetId="12" r:id="rId3"/>
     <sheet name="teabag_decomposition_data" sheetId="4" r:id="rId4"/>
     <sheet name="sedimentation_data" sheetId="11" r:id="rId5"/>
-    <sheet name="glossary" sheetId="7" r:id="rId6"/>
+    <sheet name="frame_fertilizer_presence" sheetId="13" r:id="rId6"/>
+    <sheet name="glossary" sheetId="7" r:id="rId7"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId7"/>
     <externalReference r:id="rId8"/>
+    <externalReference r:id="rId9"/>
   </externalReferences>
   <definedNames>
     <definedName name="coverType">[1]Vocab!$B$41:$B$44</definedName>
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="253">
   <si>
     <t>sheet</t>
   </si>
@@ -921,6 +922,9 @@
   <si>
     <t>sediment sample - organic matter</t>
   </si>
+  <si>
+    <t>fertilizer_presence_or_absence</t>
+  </si>
 </sst>
 </file>
 
@@ -929,7 +933,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1098,6 +1102,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1898,7 +1908,7 @@
   </sheetPr>
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -5364,6 +5374,121 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5A9447F-C1EA-4630-BF80-C92B0FB70CB7}">
+  <sheetPr>
+    <tabColor rgb="FF97C8EB"/>
+  </sheetPr>
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="40" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A1" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>252</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>246</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="25" type="noConversion"/>
+  <dataValidations count="6">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Weight, in grams of the tea bags. Please refer to the protocol for instructions for weighing the tea bags." sqref="C1" xr:uid="{51C312B0-9C82-4F02-9B76-F4AAC457DBDC}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Any additional notes regarding observations, context, or concerns about the data." sqref="E1" xr:uid="{7909C9E5-CFA4-4C85-A1B2-F2973316AEB2}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The full name of the person processing the sample (no initials; ONLY one name per sample)" sqref="D1" xr:uid="{5027D422-192D-42FA-9BEB-2BCD85159FEF}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Scientific name using standard scientific nomenclature. If the species cannot be identified to species, report genus or higher." sqref="C1" xr:uid="{9A386109-A6FF-4439-8150-16C16CFA632D}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the number of your site. Site numbers can be found in the map that you received in the package or on the MarineGEO protocol website: https://marinegeo.github.io/projects/sed-biome" sqref="A1" xr:uid="{FEB08429-490C-4D43-88E2-E8A07E51FF81}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="ID of the frame as indicated on the boyant chain and map (SiteX-C/FX)" sqref="B1" xr:uid="{05B77BDE-9D6F-4871-A9D6-CD794744115E}"/>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor rgb="FF97C8EB"/>

</xml_diff>

<commit_message>
update SED-BIOME data entry spreadsheets
</commit_message>
<xml_diff>
--- a/assets/projects/sed-biome/data-entry-spreadsheets/SED-BIOME_site-10_Australia.xlsx
+++ b/assets/projects/sed-biome/data-entry-spreadsheets/SED-BIOME_site-10_Australia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lonnemanm\Documents\repositories\marinegeo.github.io\assets\projects\sed-biome\data-entry-spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F79EA0A-415A-4E40-B6AB-78B833D034BD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{274F5CD7-3B5E-46C1-A83D-720FC2BA974B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3375" yWindow="3375" windowWidth="28800" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3885" yWindow="4065" windowWidth="28800" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="protocol_metadata" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="258">
   <si>
     <t>sheet</t>
   </si>
@@ -933,6 +933,12 @@
   </si>
   <si>
     <t>presence; absence</t>
+  </si>
+  <si>
+    <t>weight_initial_jar_g</t>
+  </si>
+  <si>
+    <t>weight_initial_jar_and_dried_sediment_g</t>
   </si>
 </sst>
 </file>
@@ -1267,35 +1273,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="11">
     <dxf>
       <fill>
         <patternFill>
@@ -1974,37 +1952,37 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A12:B1993 A10:B10 A3:B6 C1:Z1993">
-    <cfRule type="containsBlanks" dxfId="14" priority="9">
+    <cfRule type="containsBlanks" dxfId="10" priority="9">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1">
-    <cfRule type="containsBlanks" dxfId="13" priority="7">
+    <cfRule type="containsBlanks" dxfId="9" priority="7">
       <formula>LEN(TRIM(B1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:B2">
-    <cfRule type="containsBlanks" dxfId="12" priority="6">
+    <cfRule type="containsBlanks" dxfId="8" priority="6">
       <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11">
-    <cfRule type="containsBlanks" dxfId="11" priority="5">
+    <cfRule type="containsBlanks" dxfId="7" priority="5">
       <formula>LEN(TRIM(A11))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="containsBlanks" dxfId="10" priority="4">
+    <cfRule type="containsBlanks" dxfId="6" priority="4">
       <formula>LEN(TRIM(B11))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:B9">
-    <cfRule type="containsBlanks" dxfId="9" priority="3">
+    <cfRule type="containsBlanks" dxfId="5" priority="3">
       <formula>LEN(TRIM(A7))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="containsBlanks" dxfId="8" priority="1">
+    <cfRule type="containsBlanks" dxfId="4" priority="1">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4663,9 +4641,7 @@
   </sheetPr>
   <dimension ref="A1:O65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
@@ -4701,10 +4677,10 @@
         <v>92</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>93</v>
+        <v>256</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>94</v>
+        <v>257</v>
       </c>
       <c r="I1" s="16" t="s">
         <v>95</v>

</xml_diff>